<commit_message>
Added mechanical bom with fasteners etc
</commit_message>
<xml_diff>
--- a/electronics/reference/electronics_bom.xlsx
+++ b/electronics/reference/electronics_bom.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="42">
   <si>
     <t>Category</t>
   </si>
@@ -147,6 +147,9 @@
   </si>
   <si>
     <t>MOQ</t>
+  </si>
+  <si>
+    <t>Y</t>
   </si>
 </sst>
 </file>
@@ -517,7 +520,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
+      <selection pane="bottomLeft" activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -576,6 +579,9 @@
       <c r="E2">
         <v>1</v>
       </c>
+      <c r="H2" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -595,6 +601,9 @@
       <c r="B4" t="s">
         <v>12</v>
       </c>
+      <c r="H4" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
@@ -620,6 +629,9 @@
       <c r="F6">
         <v>5</v>
       </c>
+      <c r="H6" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
@@ -651,6 +663,9 @@
       <c r="F8">
         <v>5</v>
       </c>
+      <c r="H8" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
@@ -665,6 +680,9 @@
       <c r="F9">
         <v>100</v>
       </c>
+      <c r="H9" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
@@ -718,6 +736,9 @@
       <c r="F13">
         <v>10</v>
       </c>
+      <c r="H13" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
@@ -748,13 +769,16 @@
       <c r="F16">
         <v>10</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -769,6 +793,9 @@
       </c>
       <c r="F27">
         <v>100</v>
+      </c>
+      <c r="H27" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>